<commit_message>
format output info and save result in file
</commit_message>
<xml_diff>
--- a/book-list.xlsx
+++ b/book-list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Zfiles\Coder\MyRepos\book-recommendation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6AB4122-84C1-4155-B1CA-606587AE81E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15699D63-71E0-491A-ADEC-4991B67644DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" xr2:uid="{FE6CB96C-626F-492F-AF00-5035E3094679}"/>
   </bookViews>
@@ -269,10 +269,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>备注或简评</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>C语言程序设计：现代方法</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -429,10 +425,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>相关链接（通常是豆瓣链接，偶尔是源网站）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>技术，计算机组成原理，入门</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -539,6 +531,14 @@
   </si>
   <si>
     <t>我不该评级为★★★★★★，因为这本书对我来说是没法评级的。有没有一本书在你心目中，没办法和其他书相安无事地排在一起，这就是我的那本书。</t>
+  </si>
+  <si>
+    <t>相关链接</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Memo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -932,8 +932,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{756F14E8-76FA-47F5-8995-A8D87CCF1952}">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -959,10 +959,10 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>48</v>
+        <v>116</v>
       </c>
       <c r="F1" t="s">
-        <v>88</v>
+        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -970,16 +970,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D2" t="s">
+        <v>110</v>
+      </c>
+      <c r="E2" t="s">
         <v>81</v>
-      </c>
-      <c r="C2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D2" t="s">
-        <v>112</v>
-      </c>
-      <c r="E2" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -990,13 +990,13 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D3" t="s">
+        <v>82</v>
+      </c>
+      <c r="E3" t="s">
         <v>83</v>
-      </c>
-      <c r="E3" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1007,13 +1007,13 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D4" t="s">
+        <v>82</v>
+      </c>
+      <c r="E4" t="s">
         <v>83</v>
-      </c>
-      <c r="E4" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1024,13 +1024,13 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1038,16 +1038,16 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" t="s">
+        <v>111</v>
+      </c>
+      <c r="D6" t="s">
         <v>60</v>
       </c>
-      <c r="C6" t="s">
-        <v>113</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>61</v>
-      </c>
-      <c r="E6" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1058,13 +1058,13 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D7" t="s">
         <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1075,7 +1075,7 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D8" t="s">
         <v>17</v>
@@ -1089,7 +1089,7 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D9" t="s">
         <v>15</v>
@@ -1103,7 +1103,7 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D10" t="s">
         <v>15</v>
@@ -1117,7 +1117,7 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D11" t="s">
         <v>15</v>
@@ -1128,10 +1128,10 @@
         <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>15</v>
@@ -1145,7 +1145,7 @@
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D13" t="s">
         <v>16</v>
@@ -1159,7 +1159,7 @@
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D14" t="s">
         <v>16</v>
@@ -1173,7 +1173,7 @@
         <v>12</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>16</v>
@@ -1187,7 +1187,7 @@
         <v>13</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>16</v>
@@ -1201,13 +1201,13 @@
         <v>19</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="18" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1218,13 +1218,13 @@
         <v>20</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1235,13 +1235,13 @@
         <v>21</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D19" s="2" t="s">
         <v>41</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1252,7 +1252,7 @@
         <v>22</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>26</v>
@@ -1266,16 +1266,16 @@
         <v>1</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>50</v>
-      </c>
       <c r="E21" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="22" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -1286,13 +1286,13 @@
         <v>23</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>27</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1303,7 +1303,7 @@
         <v>24</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>25</v>
@@ -1320,13 +1320,13 @@
         <v>28</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1337,13 +1337,13 @@
         <v>30</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1354,7 +1354,7 @@
         <v>32</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>33</v>
@@ -1371,7 +1371,7 @@
         <v>34</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D27" s="2" t="s">
         <v>35</v>
@@ -1388,7 +1388,7 @@
         <v>36</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D28" s="2" t="s">
         <v>37</v>
@@ -1405,13 +1405,13 @@
         <v>38</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1422,13 +1422,13 @@
         <v>39</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D30" s="2" t="s">
         <v>40</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1436,16 +1436,16 @@
         <v>1</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D31" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E31" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="E31" s="2" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1453,13 +1453,13 @@
         <v>1</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D32" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="C32" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D32" s="2" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1467,16 +1467,16 @@
         <v>1</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="C33" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="E33" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1484,16 +1484,16 @@
         <v>1</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1501,16 +1501,16 @@
         <v>0</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="E35" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1518,16 +1518,16 @@
         <v>1</v>
       </c>
       <c r="B36" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D36" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="C36" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D36" s="2" t="s">
+      <c r="E36" s="2" t="s">
         <v>79</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>80</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1535,16 +1535,16 @@
         <v>1</v>
       </c>
       <c r="B37" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D37" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C37" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="D37" s="2" t="s">
+      <c r="E37" s="2" t="s">
         <v>86</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1552,16 +1552,16 @@
         <v>1</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1569,16 +1569,16 @@
         <v>1</v>
       </c>
       <c r="B39" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E39" t="s">
         <v>92</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E39" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1586,13 +1586,13 @@
         <v>1</v>
       </c>
       <c r="B40" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D40" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1600,16 +1600,16 @@
         <v>1</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1617,16 +1617,16 @@
         <v>1</v>
       </c>
       <c r="B42" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="E42" s="2" t="s">
         <v>109</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1634,13 +1634,13 @@
         <v>1</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1648,13 +1648,13 @@
         <v>1</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1662,13 +1662,13 @@
         <v>1</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1676,13 +1676,13 @@
         <v>1</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add links, rename and update README
</commit_message>
<xml_diff>
--- a/book-list.xlsx
+++ b/book-list.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Zfiles\Coder\MyRepos\book-recommendation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15699D63-71E0-491A-ADEC-4991B67644DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE7AF518-810B-4618-99CF-0C1F27558C6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" xr2:uid="{FE6CB96C-626F-492F-AF00-5035E3094679}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="158">
   <si>
     <t>图书名</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -213,10 +213,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>程序员面试宝典</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>技术，算法与数据结构，Java，入门，初级</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -329,10 +325,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>代码整洁之道</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>算法图解</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -369,10 +361,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>与《重构》二读其一即可，我选的《重构》，这本只读了前面几章，主题相同。（其实和《代码大全》暗合，时间有限时三本里看一本也是可以的。）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>补足了C语言圣经的一个缺陷：那本书用的C语言版本有点老，这本新点。时间有限时可以二选一选这本，但C圣经很薄的，没必要抛弃。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -441,10 +429,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>阅读是一所随身携带的避难所</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>李存捧的译本个人认为最佳。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -530,22 +514,159 @@
     <t>★★★★★★</t>
   </si>
   <si>
-    <t>我不该评级为★★★★★★，因为这本书对我来说是没法评级的。有没有一本书在你心目中，没办法和其他书相安无事地排在一起，这就是我的那本书。</t>
-  </si>
-  <si>
     <t>相关链接</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Memo</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://book.douban.com/subject/4163938/</t>
+  </si>
+  <si>
+    <t>https://book.douban.com/subject/6860890/</t>
+  </si>
+  <si>
+    <t>https://book.douban.com/subject/6021440/</t>
+  </si>
+  <si>
+    <t>https://book.douban.com/subject/25881855/</t>
+  </si>
+  <si>
+    <t>https://book.douban.com/subject/30320887/</t>
+  </si>
+  <si>
+    <t>https://book.douban.com/subject/1037602/</t>
+  </si>
+  <si>
+    <t>https://book.douban.com/subject/25930025/</t>
+  </si>
+  <si>
+    <t>https://book.douban.com/subject/5414391/</t>
+  </si>
+  <si>
+    <t>https://book.douban.com/subject/26818878/</t>
+  </si>
+  <si>
+    <t>https://book.douban.com/subject/1027191/</t>
+  </si>
+  <si>
+    <t>https://book.douban.com/subject/1041482/</t>
+  </si>
+  <si>
+    <t>https://book.douban.com/subject/30175059/</t>
+  </si>
+  <si>
+    <t>https://book.douban.com/subject/25985021/</t>
+  </si>
+  <si>
+    <t>https://book.douban.com/subject/30259720/</t>
+  </si>
+  <si>
+    <t>https://book.douban.com/subject/26943161/</t>
+  </si>
+  <si>
+    <t>https://book.douban.com/subject/6518605/</t>
+  </si>
+  <si>
+    <t>https://book.douban.com/subject/4822685/</t>
+  </si>
+  <si>
+    <t>https://book.douban.com/subject/26912767/</t>
+  </si>
+  <si>
+    <t>https://book.douban.com/subject/1139336/</t>
+  </si>
+  <si>
+    <t>https://book.douban.com/subject/35503091/</t>
+  </si>
+  <si>
+    <t>https://book.douban.com/subject/2778632/</t>
+  </si>
+  <si>
+    <t>https://book.douban.com/subject/27028517/</t>
+  </si>
+  <si>
+    <t>https://book.douban.com/subject/34898994/</t>
+  </si>
+  <si>
+    <t>https://book.douban.com/subject/2130190/</t>
+  </si>
+  <si>
+    <t>https://book.douban.com/subject/26854244/</t>
+  </si>
+  <si>
+    <t>程序员面试金典</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://book.douban.com/subject/34813624/</t>
+  </si>
+  <si>
+    <t>https://book.douban.com/subject/33463930/</t>
+  </si>
+  <si>
+    <t>https://book.douban.com/subject/35175321/</t>
+  </si>
+  <si>
+    <t>https://book.douban.com/subject/30280001/</t>
+  </si>
+  <si>
+    <t>https://book.douban.com/subject/1477390/</t>
+  </si>
+  <si>
+    <t>https://book.douban.com/subject/26979890/</t>
+  </si>
+  <si>
+    <t>https://book.douban.com/subject/30468597/</t>
+  </si>
+  <si>
+    <t>https://book.douban.com/subject/26857423/</t>
+  </si>
+  <si>
+    <t>https://book.douban.com/subject/3354490/</t>
+  </si>
+  <si>
+    <t>https://billie66.github.io/TLCL/</t>
+  </si>
+  <si>
+    <t>https://book.douban.com/subject/27614904/</t>
+  </si>
+  <si>
+    <t>https://book.douban.com/subject/6042374/</t>
+  </si>
+  <si>
+    <t>阅读是一座随身携带的避难所</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>https://book.douban.com/subject/27024398/</t>
+  </si>
+  <si>
+    <t>https://book.douban.com/subject/6952036/</t>
+  </si>
+  <si>
+    <t>https://book.douban.com/subject/30545322/</t>
+  </si>
+  <si>
+    <t>https://book.douban.com/subject/25976544/</t>
+  </si>
+  <si>
+    <t>https://book.douban.com/subject/1033778/</t>
+  </si>
+  <si>
+    <t>https://book.douban.com/subject/27170538/</t>
+  </si>
+  <si>
+    <t>https://book.douban.com/subject/1066462/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -583,6 +704,13 @@
       <family val="3"/>
       <charset val="134"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="楷体"/>
+      <family val="3"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -606,7 +734,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -614,6 +742,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -930,24 +1061,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{756F14E8-76FA-47F5-8995-A8D87CCF1952}">
-  <dimension ref="A1:F46"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="34.6640625" customWidth="1"/>
-    <col min="3" max="3" width="12.77734375" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="51.5546875" customWidth="1"/>
     <col min="5" max="5" width="177.6640625" customWidth="1"/>
-    <col min="6" max="6" width="62.77734375" customWidth="1"/>
+    <col min="6" max="6" width="41.5546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -959,10 +1090,10 @@
         <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="F1" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -970,16 +1101,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D2" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E2" t="s">
-        <v>81</v>
+        <v>78</v>
+      </c>
+      <c r="F2" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -990,13 +1124,16 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D3" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E3" t="s">
-        <v>83</v>
+        <v>80</v>
+      </c>
+      <c r="F3" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1007,13 +1144,16 @@
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E4" t="s">
-        <v>83</v>
+        <v>80</v>
+      </c>
+      <c r="F4" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1024,13 +1164,16 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D5" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E5" t="s">
-        <v>55</v>
+        <v>54</v>
+      </c>
+      <c r="F5" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -1038,16 +1181,19 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D6" t="s">
         <v>59</v>
       </c>
-      <c r="C6" t="s">
-        <v>111</v>
-      </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>60</v>
       </c>
-      <c r="E6" t="s">
-        <v>61</v>
+      <c r="F6" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1058,13 +1204,16 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D7" t="s">
         <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>62</v>
+        <v>61</v>
+      </c>
+      <c r="F7" t="s">
+        <v>117</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -1075,11 +1224,14 @@
         <v>6</v>
       </c>
       <c r="C8" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D8" t="s">
         <v>17</v>
       </c>
+      <c r="F8" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -1089,11 +1241,14 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D9" t="s">
         <v>15</v>
       </c>
+      <c r="F9" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -1103,11 +1258,14 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D10" t="s">
         <v>15</v>
       </c>
+      <c r="F10" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -1117,25 +1275,31 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D11" t="s">
         <v>15</v>
       </c>
+      <c r="F11" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="F12" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -1145,11 +1309,14 @@
         <v>10</v>
       </c>
       <c r="C13" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D13" t="s">
         <v>16</v>
       </c>
+      <c r="F13" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -1159,11 +1326,14 @@
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D14" t="s">
         <v>16</v>
       </c>
+      <c r="F14" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="15" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -1173,11 +1343,14 @@
         <v>12</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="F15" s="2" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="16" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16">
@@ -1187,13 +1360,16 @@
         <v>13</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F16" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>1</v>
       </c>
@@ -1201,16 +1377,19 @@
         <v>19</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
@@ -1218,16 +1397,19 @@
         <v>20</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>51</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1</v>
       </c>
@@ -1235,16 +1417,19 @@
         <v>21</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1</v>
       </c>
@@ -1252,33 +1437,39 @@
         <v>22</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D20" s="2" t="s">
         <v>26</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>1</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="C21" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D21" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="E21" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>1</v>
       </c>
@@ -1286,16 +1477,19 @@
         <v>23</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D22" s="2" t="s">
         <v>27</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+        <v>49</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>1</v>
       </c>
@@ -1303,16 +1497,19 @@
         <v>24</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>25</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+        <v>42</v>
+      </c>
+      <c r="F23" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>1</v>
       </c>
@@ -1320,16 +1517,19 @@
         <v>28</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D24" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+        <v>52</v>
+      </c>
+      <c r="F24" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>1</v>
       </c>
@@ -1337,16 +1537,19 @@
         <v>30</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D25" s="2" t="s">
         <v>31</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="F25" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>1</v>
       </c>
@@ -1354,335 +1557,376 @@
         <v>32</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E26" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F26" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E27" s="2" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>1</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D27" s="2" t="s">
+      <c r="F27" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="E27" s="2" t="s">
+      <c r="C28" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E28" s="2" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>1</v>
-      </c>
-      <c r="B28" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D28" s="2" t="s">
+      <c r="F28" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E28" s="2" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>1</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>38</v>
-      </c>
       <c r="C29" s="2" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>33</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+        <v>69</v>
+      </c>
+      <c r="F29" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>1</v>
       </c>
       <c r="B30" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D30" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>40</v>
-      </c>
       <c r="E30" s="2" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+      <c r="F30" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>1</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+      <c r="F31" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>1</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F32" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="C32" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D32" s="2" t="s">
+      <c r="C33" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D33" s="2" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>1</v>
-      </c>
-      <c r="B33" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="C33" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D33" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="E33" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F33" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>0</v>
+      </c>
+      <c r="B34" s="2" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>1</v>
-      </c>
-      <c r="B34" s="2" t="s">
-        <v>63</v>
-      </c>
       <c r="C34" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+      <c r="F34" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B35" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C35" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D35" s="2" t="s">
+      <c r="E35" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E35" s="2" t="s">
+      <c r="F35" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="F36" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="14.4" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E37" s="2"/>
+      <c r="F37" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E38" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>1</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="C36" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D36" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="E36" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>1</v>
-      </c>
-      <c r="B37" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C37" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D37" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E37" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>1</v>
-      </c>
-      <c r="B38" s="2" t="s">
+      <c r="F38" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>1</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D39" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C38" s="2" t="s">
-        <v>113</v>
-      </c>
-      <c r="D38" s="2" t="s">
+      <c r="F39" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>1</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="F40" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="F41" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <v>1</v>
+      </c>
+      <c r="B42" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E38" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>1</v>
-      </c>
-      <c r="B39" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C39" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="E39" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>1</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>1</v>
-      </c>
-      <c r="B41" s="2" t="s">
+      <c r="C42" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F42" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <v>1</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D43" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C41" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D41" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E41" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>1</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="C42" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D42" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>1</v>
-      </c>
-      <c r="B43" s="2" t="s">
+      <c r="F43" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <v>1</v>
+      </c>
+      <c r="B44" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C43" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D43" s="2" t="s">
+      <c r="C44" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>99</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>1</v>
-      </c>
-      <c r="B44" s="2" t="s">
+      <c r="F44" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <v>1</v>
+      </c>
+      <c r="B45" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C44" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D44" s="2" t="s">
+      <c r="C45" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="D45" s="2" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>1</v>
-      </c>
-      <c r="B45" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>1</v>
-      </c>
-      <c r="B46" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>105</v>
+      <c r="F45" t="s">
+        <v>157</v>
       </c>
     </row>
   </sheetData>

</xml_diff>